<commit_message>
made changes to scirpt 2 for kpack functions
</commit_message>
<xml_diff>
--- a/Resources/KPack.xlsx
+++ b/Resources/KPack.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>UID</t>
   </si>
@@ -28,6 +28,15 @@
   </si>
   <si>
     <t>Password#1</t>
+  </si>
+  <si>
+    <t>siva's id</t>
+  </si>
+  <si>
+    <t>ramya's id</t>
+  </si>
+  <si>
+    <t>DCATEST4</t>
   </si>
 </sst>
 </file>
@@ -366,19 +375,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -386,12 +396,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>